<commit_message>
adicionando fontes aos parâmetros. todos os parâmetros tem sustentação
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="265">
   <si>
     <t>Variavel</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Não utilizado.</t>
   </si>
   <si>
-    <t>Este parâmetro não é utilizado com a formulação de inicialização dos estoques atual.</t>
-  </si>
-  <si>
     <t>aReferencePrice</t>
   </si>
   <si>
@@ -257,18 +254,12 @@
     <t>Fração de Consumidores Inovadores</t>
   </si>
   <si>
-    <t>Não há base para definição deste parâmetro. Adotado o valor arbitrado por Sterman, com um fator de variação 5.</t>
-  </si>
-  <si>
     <t>aWOMStrength</t>
   </si>
   <si>
     <t>Força da Difusão do Produto “Boca a Boca”</t>
   </si>
   <si>
-    <t>Utilizado o range testado por Sterman.</t>
-  </si>
-  <si>
     <t>aPopulation</t>
   </si>
   <si>
@@ -432,9 +423,6 @@
   </si>
   <si>
     <t>$ / patente</t>
-  </si>
-  <si>
-    <t>Calculado considerando todo o investimento observado em P&amp;D da 3D Systems, dividido pelo número de patentes indicado no relatório do Gov. Britânico (90)</t>
   </si>
   <si>
     <t>aTempoMedioAvaliacao</t>
@@ -773,18 +761,12 @@
     <t>Fontes Utilizadas</t>
   </si>
   <si>
-    <t>(STERMAN 2007)</t>
-  </si>
-  <si>
     <t>Manteve-se o parâmetro definido por Sterman (2007).</t>
   </si>
   <si>
     <t>(ERNST &amp; YOUNG GMBH, 2016)</t>
   </si>
   <si>
-    <t>Estimado</t>
-  </si>
-  <si>
     <t>O Market Share Inicial das empresas considera que três empresas (3D Systems, Stratasys e EOS) dominam 70% do mercado (ERNST &amp; YOUNG GMBH, 2016, p. 54).</t>
   </si>
   <si>
@@ -812,9 +794,6 @@
     <t>Este parâmetro é apenas utilizado pelo modelo como um batente mínimo para a capacidade. O valor definido neste parâmetro serve como um valor de capacidade mínimo, abaixo do qual a capacidade da empresa não pode ser definida. Será arbitrado o valor 120 para que nenhum player possa ter capacidade produtiva menor do que 1% do mercado (aproximadamente 12000 no ano inicial).</t>
   </si>
   <si>
-    <t>O módulo PeD deve ser considerado na análise.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Considerado como 18, visto que, no modelo, a patente </t>
   </si>
   <si>
@@ -828,6 +807,75 @@
   </si>
   <si>
     <t>Como referência, adotou-se o valor de performance máximo.</t>
+  </si>
+  <si>
+    <t>O módulo PeD deve ser ativado na análise.</t>
+  </si>
+  <si>
+    <t>Variável não utilizada.</t>
+  </si>
+  <si>
+    <t>Utilizou-se a última informação disponível sobre o número de impressoras 3D profissionais vendidas como referência para calibrar as condições iniciais do modelo.</t>
+  </si>
+  <si>
+    <t>Wholers (achar)</t>
+  </si>
+  <si>
+    <t>Arbitrado o valor de 0,7 a 1, pressupondo que o custo será reduzido em 30% caso a empresa produza a mesma quantidade de produtos vendidos inicialmente.</t>
+  </si>
+  <si>
+    <t>Não há fonte de informação para definição deste parâmetro. Adotado o valor arbitrado por Sterman, com um fator de variação 10.</t>
+  </si>
+  <si>
+    <t>Calculado considerando todo o investimento observado em P&amp;D da 3D Systems, dividido pelo número de patentes de posse da 3D systems observado.</t>
+  </si>
+  <si>
+    <t>Tentar fazer busca de patentes pela 3D systems, e olhar apenas patentes ganhas nos últios 5 anos.</t>
+  </si>
+  <si>
+    <t>O tempo médio de avaliação foi considerado como incerto, variando de 1,5 a 3 anos. A média observada é de 1 ano e 8 meses).</t>
+  </si>
+  <si>
+    <t>A Taxa de rejeição média calculada foi de 0,4. Esta variável também foi considerada como incerta, devido ao fato de que o crescimento do número de patentes emitidas pode aumentar esta taxa ao longo do tempo.</t>
+  </si>
+  <si>
+    <t>Considera-se que uma patente em donmínio público não será útil (ou seja, não gerará performance) idenfinidamente. Foram arbitrados tempos máximos e mínimos para esta variável.</t>
+  </si>
+  <si>
+    <t>Arbitrado.</t>
+  </si>
+  <si>
+    <t>(QUANDL, 2017)</t>
+  </si>
+  <si>
+    <t>Não há informação disponível para determinar a fração inicial de pedidos que é oriúnda de substituições de impressoras 3D em fim de vida útil.</t>
+  </si>
+  <si>
+    <t>Variável considerada como incerta, pressupondo que os players podem optar por tornar todo o seu investimento em Patentes Open Source.</t>
+  </si>
+  <si>
+    <t>(STERMAN, 2007)</t>
+  </si>
+  <si>
+    <t>Utilizado o range testado por Sterman (2007).</t>
+  </si>
+  <si>
+    <t>Param. Original</t>
+  </si>
+  <si>
+    <t>Estim. Dados Obs.</t>
+  </si>
+  <si>
+    <t>Foi considerado que o player tem a mesma liberdade de decisão que o player analisado, variando seu market share desejado em 1/3 a mais ou a menos do que seu market share inicial.</t>
+  </si>
+  <si>
+    <t>Foi considerado que o player tem a mesma liberdade de decisão que o player analisado, podendo optar por uma estratégia agressiva ou conservadora. Os ranges de variam entre 0,5 e 2,5 para que, ao arredondados, os valores 1 e 2 tenham a mesma probabilidade de ocorrência.</t>
+  </si>
+  <si>
+    <t>Não há informações disponíveis sobre empresas que atuem no ramo de impressoras profissionais com patentes open source.</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1733,14 +1781,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AMJ80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,10 +1860,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="R1" t="s">
         <v>15</v>
@@ -1875,10 +1922,10 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>10</v>
+        <v>259</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R2" t="s">
         <v>22</v>
@@ -1935,11 +1982,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>10</v>
+      <c r="P3" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q3" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -1996,11 +2043,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>10</v>
+      <c r="P4" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q4" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R4" t="s">
         <v>30</v>
@@ -2057,11 +2104,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>10</v>
+      <c r="P5" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q5" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R5" t="s">
         <v>34</v>
@@ -2072,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -2128,7 +2175,9 @@
       <c r="P6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q6" s="17"/>
+      <c r="Q6" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R6" t="s">
         <v>40</v>
       </c>
@@ -2187,9 +2236,11 @@
       <c r="P7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="17"/>
+      <c r="Q7" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R7" t="s">
-        <v>45</v>
+        <v>243</v>
       </c>
       <c r="S7"/>
       <c r="T7" s="1" t="b">
@@ -2199,10 +2250,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="C8" s="7">
         <f t="shared" si="0"/>
@@ -2213,7 +2264,7 @@
         <v>107000</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="7">
         <v>0.5</v>
@@ -2244,13 +2295,13 @@
         <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="S8" s="1">
         <f>107/0.5</f>
@@ -2261,12 +2312,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
@@ -2277,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
@@ -2311,26 +2362,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>10</v>
+      <c r="P9" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T9" s="1" t="b">
         <f>J9=[1]params_testeithink!J9</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="C10" s="10">
         <f t="shared" si="0"/>
@@ -2341,7 +2392,7 @@
         <v>100000</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="10">
         <v>1</v>
@@ -2376,21 +2427,23 @@
       <c r="P10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q10" s="17"/>
+      <c r="Q10" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T10" s="1" t="b">
         <f>J10=[1]params_testeithink!J10</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C11" s="12">
         <f t="shared" si="0"/>
@@ -2431,26 +2484,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>10</v>
+      <c r="P11" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R11" t="s">
-        <v>59</v>
+        <v>247</v>
       </c>
       <c r="T11" s="1" t="b">
         <f>J11=[1]params_testeithink!J11</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
@@ -2461,7 +2514,7 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="2">
         <v>6</v>
@@ -2495,14 +2548,14 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>10</v>
+      <c r="P12" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R12" t="s">
-        <v>62</v>
+        <v>257</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="T12" s="1" t="b">
         <f>J12=[1]params_testeithink!J12</f>
@@ -2511,10 +2564,10 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C13" s="10">
         <f>D10</f>
@@ -2525,7 +2578,7 @@
         <v>100000</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="10">
         <v>5</v>
@@ -2560,9 +2613,11 @@
       <c r="P13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q13" s="17"/>
+      <c r="Q13" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="T13" s="1" t="b">
         <f>J13=[1]params_testeithink!J13</f>
@@ -2571,10 +2626,10 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ref="C14:C22" si="4">IF(I14="Incerto",MAX(G14,J14-(ABS(F14*J14))),J14)</f>
@@ -2613,26 +2668,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>10</v>
+      <c r="P14" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q14" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R14" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T14" s="1" t="b">
         <f>J14=[1]params_testeithink!J14</f>
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="4"/>
@@ -2679,13 +2734,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>10</v>
+      <c r="P15" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q15" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R15"/>
+        <v>257</v>
+      </c>
+      <c r="R15" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T15" s="1" t="b">
         <f>J15=[1]params_testeithink!J15</f>
         <v>1</v>
@@ -2693,10 +2750,10 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="4"/>
@@ -2737,26 +2794,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>10</v>
+      <c r="P16" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q16" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T16" s="1" t="b">
         <f>J16=[1]params_testeithink!J16</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="4"/>
@@ -2801,13 +2858,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>10</v>
+      <c r="P17" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q17" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R17"/>
+        <v>257</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T17" s="1" t="b">
         <f>J17=[1]params_testeithink!J17</f>
         <v>1</v>
@@ -2815,10 +2874,10 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="4"/>
@@ -2859,14 +2918,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>10</v>
+      <c r="P18" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q18" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T18" s="1" t="b">
         <f>J18=[1]params_testeithink!J18</f>
@@ -2875,10 +2934,10 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="4"/>
@@ -2919,26 +2978,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>10</v>
+      <c r="P19" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q19" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T19" s="1" t="b">
         <f>J19=[1]params_testeithink!J19</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="4"/>
@@ -2979,26 +3038,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>10</v>
+      <c r="P20" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q20" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="T20" s="1" t="b">
         <f>J20=[1]params_testeithink!J20</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="4"/>
@@ -3043,24 +3102,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>10</v>
+      <c r="P21" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q21" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R21"/>
+        <v>257</v>
+      </c>
+      <c r="R21" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T21" s="1" t="b">
         <f>J21=[1]params_testeithink!J21</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="4"/>
@@ -3104,7 +3165,12 @@
       <c r="P22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R22"/>
+      <c r="Q22" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R22" t="s">
+        <v>246</v>
+      </c>
       <c r="T22" s="1" t="b">
         <f>J22=[1]params_testeithink!J22</f>
         <v>1</v>
@@ -3112,10 +3178,10 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2">
         <f>IF(H23="Incerto",MAX(G23,J23-(ABS(F23*J23))),J23)</f>
@@ -3126,7 +3192,7 @@
         <v>100000</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F23" s="2">
         <v>0.5</v>
@@ -3161,20 +3227,23 @@
       <c r="P23" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q23" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T23" s="1" t="b">
         <f>J23=[1]params_testeithink!J23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" ref="C24:C55" si="6">IF(I24="Incerto",MAX(G24,J24-(ABS(F24*J24))),J24)</f>
@@ -3220,13 +3289,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>10</v>
+      <c r="P24" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q24" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R24"/>
+        <v>257</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T24" s="1" t="b">
         <f>J24=[1]params_testeithink!J24</f>
         <v>1</v>
@@ -3234,10 +3305,10 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="6"/>
@@ -3278,26 +3349,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>10</v>
+      <c r="P25" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q25" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T25" s="1" t="b">
         <f>J25=[1]params_testeithink!J25</f>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="6"/>
@@ -3342,13 +3413,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>10</v>
+      <c r="P26" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q26" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R26"/>
+        <v>257</v>
+      </c>
+      <c r="R26" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T26" s="1" t="b">
         <f>J26=[1]params_testeithink!J26</f>
         <v>1</v>
@@ -3356,10 +3429,10 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="6"/>
@@ -3370,7 +3443,7 @@
         <v>200</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F27" s="2">
         <v>0.5</v>
@@ -3405,24 +3478,27 @@
       <c r="P27" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q27" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R27" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="T27" s="1" t="b">
         <f>J27=[1]params_testeithink!J27</f>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="7"/>
@@ -3439,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="J28" s="1">
         <v>1</v>
@@ -3451,17 +3527,21 @@
       <c r="M28"/>
       <c r="N28" s="1" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="1" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q28" s="18"/>
-      <c r="R28"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q28" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="R28" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T28" s="1" t="b">
         <f>J28=[1]params_testeithink!J28</f>
         <v>1</v>
@@ -3469,10 +3549,10 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="6"/>
@@ -3513,14 +3593,14 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>10</v>
+      <c r="P29" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q29" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T29" s="1" t="b">
         <f>J29=[1]params_testeithink!J29</f>
@@ -3529,10 +3609,10 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="6"/>
@@ -3573,26 +3653,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>10</v>
+      <c r="P30" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q30" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T30" s="1" t="b">
         <f>J30=[1]params_testeithink!J30</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="6"/>
@@ -3637,24 +3717,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>10</v>
+      <c r="P31" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q31" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R31"/>
+        <v>257</v>
+      </c>
+      <c r="R31" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T31" s="1" t="b">
         <f>J31=[1]params_testeithink!J31</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="6"/>
@@ -3699,24 +3781,26 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>10</v>
+      <c r="P32" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q32" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R32"/>
+        <v>257</v>
+      </c>
+      <c r="R32" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T32" s="1" t="b">
         <f>J32=[1]params_testeithink!J32</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="6"/>
@@ -3761,13 +3845,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="P33" s="1" t="s">
-        <v>10</v>
+      <c r="P33" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q33" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="R33"/>
+        <v>257</v>
+      </c>
+      <c r="R33" s="17" t="s">
+        <v>258</v>
+      </c>
       <c r="T33" s="1" t="b">
         <f>J33=[1]params_testeithink!J33</f>
         <v>1</v>
@@ -3775,10 +3861,10 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="6"/>
@@ -3819,14 +3905,14 @@
         <f t="shared" ref="O34:O70" si="8">D34&gt;C34</f>
         <v>0</v>
       </c>
-      <c r="P34" s="1" t="s">
-        <v>10</v>
+      <c r="P34" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="Q34" s="18" t="s">
-        <v>230</v>
+        <v>257</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="T34" s="1" t="b">
         <f>J34=[1]params_testeithink!J34</f>
@@ -3835,10 +3921,10 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="6"/>
@@ -3879,28 +3965,31 @@
       <c r="P35" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q35" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="T35" s="1" t="b">
         <f>J35=[1]params_testeithink!J35</f>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>29</v>
@@ -3918,10 +4007,10 @@
         <v>38</v>
       </c>
       <c r="J36" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K36" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L36"/>
       <c r="M36"/>
@@ -3933,18 +4022,23 @@
       <c r="P36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R36"/>
+      <c r="Q36" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R36" t="s">
+        <v>253</v>
+      </c>
       <c r="T36" s="1" t="b">
         <f>J36=[1]params_testeithink!J36</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="6"/>
@@ -3955,7 +4049,7 @@
         <v>5805133.3333333349</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F37" s="2">
         <v>0.5</v>
@@ -3985,23 +4079,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P37" s="1" t="s">
-        <v>39</v>
+      <c r="P37" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q37" s="18" t="s">
+        <v>249</v>
       </c>
       <c r="R37" t="s">
-        <v>118</v>
+        <v>248</v>
       </c>
       <c r="T37" s="1" t="b">
         <f>J37=[1]params_testeithink!J37</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="6"/>
@@ -4040,21 +4137,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R38"/>
+      <c r="P38" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q38" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="R38" t="s">
+        <v>250</v>
+      </c>
       <c r="T38" s="1" t="b">
         <f>J38=[1]params_testeithink!J38</f>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C39" s="2">
         <f t="shared" si="6"/>
@@ -4065,7 +4167,7 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F39" s="2">
         <v>0.5</v>
@@ -4092,10 +4194,15 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R39"/>
+      <c r="P39" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q39" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="R39" t="s">
+        <v>251</v>
+      </c>
       <c r="T39" s="1" t="b">
         <f>J39=[1]params_testeithink!J39</f>
         <v>1</v>
@@ -4103,10 +4210,10 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C40" s="2">
         <f t="shared" si="6"/>
@@ -4146,26 +4253,26 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P40" s="1" t="s">
-        <v>39</v>
+      <c r="P40" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="Q40" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="R40" t="s">
         <v>237</v>
-      </c>
-      <c r="R40" t="s">
-        <v>244</v>
       </c>
       <c r="T40" s="1" t="b">
         <f>J40=[1]params_testeithink!J40</f>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C41" s="2">
         <f t="shared" si="6"/>
@@ -4208,18 +4315,23 @@
       <c r="P41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R41"/>
+      <c r="Q41" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R41" t="s">
+        <v>252</v>
+      </c>
       <c r="T41" s="1" t="b">
         <f>J41=[1]params_testeithink!J41</f>
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C42" s="2">
         <f t="shared" si="6"/>
@@ -4230,7 +4342,7 @@
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F42" s="2">
         <v>0.5</v>
@@ -4264,7 +4376,12 @@
       <c r="P42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R42"/>
+      <c r="Q42" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R42" t="s">
+        <v>253</v>
+      </c>
       <c r="T42" s="1" t="b">
         <f>J42=[1]params_testeithink!J42</f>
         <v>0</v>
@@ -4272,10 +4389,10 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C43" s="2">
         <f t="shared" si="6"/>
@@ -4313,14 +4430,14 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P43" s="1" t="s">
-        <v>233</v>
+      <c r="P43" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="Q43" s="18" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="R43" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="T43" s="1" t="b">
         <f>J43=[1]params_testeithink!J43</f>
@@ -4329,10 +4446,10 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C44" s="2">
         <f t="shared" si="6"/>
@@ -4370,23 +4487,23 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P44" s="1" t="s">
-        <v>233</v>
+      <c r="P44" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="Q44" s="18" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="T44" s="1" t="b">
         <f>J44=[1]params_testeithink!J44</f>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B45"/>
       <c r="C45" s="2">
@@ -4426,8 +4543,11 @@
       <c r="P45" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q45" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R45" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="T45" s="1" t="b">
         <f>J45=[1]params_testeithink!J45</f>
@@ -4436,7 +4556,7 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B46"/>
       <c r="C46" s="2">
@@ -4475,23 +4595,23 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P46" s="1" t="s">
-        <v>39</v>
+      <c r="P46" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="Q46" s="18" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="R46" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="T46" s="1" t="b">
         <f>J46=[1]params_testeithink!J46</f>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="2">
@@ -4531,11 +4651,14 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P47" s="1" t="s">
-        <v>39</v>
+      <c r="P47" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q47" s="18" t="s">
+        <v>254</v>
       </c>
       <c r="R47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="T47" s="1" t="b">
         <f>J47=[1]params_testeithink!J47</f>
@@ -4544,7 +4667,7 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B48"/>
       <c r="C48" s="2">
@@ -4585,13 +4708,13 @@
         <v>0</v>
       </c>
       <c r="P48" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R48" t="s">
         <v>233</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="R48" t="s">
-        <v>239</v>
       </c>
       <c r="T48" s="1" t="b">
         <f>J48=[1]params_testeithink!J48</f>
@@ -4600,7 +4723,7 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B49"/>
       <c r="C49" s="2">
@@ -4641,22 +4764,22 @@
         <v>0</v>
       </c>
       <c r="P49" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q49" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="R49" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="T49" s="1" t="b">
         <f>J49=[1]params_testeithink!J49</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B50"/>
       <c r="C50" s="2">
@@ -4698,17 +4821,20 @@
       <c r="P50" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q50" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R50" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="T50" s="1" t="b">
         <f>J50=[1]params_testeithink!J50</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B51"/>
       <c r="C51" s="2">
@@ -4748,20 +4874,23 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P51" s="1" t="s">
-        <v>39</v>
+      <c r="P51" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q51" s="18" t="s">
+        <v>254</v>
       </c>
       <c r="R51" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="T51" s="1" t="b">
         <f>J51=[1]params_testeithink!J51</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B52"/>
       <c r="C52" s="2">
@@ -4799,7 +4928,12 @@
       <c r="P52" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R52"/>
+      <c r="Q52" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R52" t="s">
+        <v>255</v>
+      </c>
       <c r="T52" s="1" t="b">
         <f>J52=[1]params_testeithink!J52</f>
         <v>1</v>
@@ -4807,7 +4941,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="7">
@@ -4845,10 +4979,15 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P53" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="R53"/>
+      <c r="P53" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q53" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R53" t="s">
+        <v>243</v>
+      </c>
       <c r="T53" s="1" t="b">
         <f>J53=[1]params_testeithink!J53</f>
         <v>0</v>
@@ -4856,7 +4995,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="7">
@@ -4893,10 +5032,15 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P54" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R54"/>
+      <c r="P54" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q54" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="R54" t="s">
+        <v>244</v>
+      </c>
       <c r="T54" s="1" t="b">
         <f>J54=[1]params_testeithink!J54</f>
         <v>0</v>
@@ -4904,7 +5048,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B55"/>
       <c r="C55" s="2">
@@ -4916,7 +5060,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F55" s="2">
         <v>0.5</v>
@@ -4941,14 +5085,14 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P55" s="1" t="s">
-        <v>233</v>
+      <c r="P55" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R55" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="T55" s="1" t="b">
         <f>J55=[1]params_testeithink!J55</f>
@@ -4957,7 +5101,7 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B56"/>
       <c r="C56" s="2">
@@ -4969,7 +5113,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F56" s="2">
         <v>0.5</v>
@@ -4995,13 +5139,13 @@
         <v>0</v>
       </c>
       <c r="P56" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q56" s="18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R56" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T56" s="1" t="b">
         <f>J56=[1]params_testeithink!J56</f>
@@ -5010,7 +5154,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B57"/>
       <c r="C57" s="2">
@@ -5022,7 +5166,7 @@
         <v>0.15</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F57" s="2">
         <v>0.5</v>
@@ -5048,13 +5192,13 @@
         <v>0</v>
       </c>
       <c r="P57" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q57" s="18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R57" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T57" s="1" t="b">
         <f>J57=[1]params_testeithink!J57</f>
@@ -5063,7 +5207,7 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B58"/>
       <c r="C58" s="2">
@@ -5075,7 +5219,7 @@
         <v>0.27999999999999992</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F58" s="2">
         <v>0.5</v>
@@ -5102,13 +5246,13 @@
         <v>0</v>
       </c>
       <c r="P58" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q58" s="18" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="R58" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T58" s="1" t="b">
         <f>J58=[1]params_testeithink!J58</f>
@@ -5117,10 +5261,10 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C59" s="2">
         <f t="shared" si="11"/>
@@ -5131,7 +5275,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F59" s="2">
         <v>0.5</v>
@@ -5160,13 +5304,13 @@
         <v>0</v>
       </c>
       <c r="P59" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q59" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="R59" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="T59" s="1" t="b">
         <f>J59=[1]params_testeithink!J59</f>
@@ -5175,7 +5319,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B60"/>
       <c r="C60" s="2">
@@ -5187,7 +5331,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F60" s="2">
         <v>0.5</v>
@@ -5214,13 +5358,13 @@
         <v>0</v>
       </c>
       <c r="P60" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q60" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="R60" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T60" s="1" t="b">
         <f>J60=[1]params_testeithink!J60</f>
@@ -5229,7 +5373,7 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B61"/>
       <c r="C61" s="2">
@@ -5241,7 +5385,7 @@
         <v>0.15</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F61" s="2">
         <v>0.5</v>
@@ -5268,13 +5412,13 @@
         <v>0</v>
       </c>
       <c r="P61" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q61" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="R61" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T61" s="1" t="b">
         <f>J61=[1]params_testeithink!J61</f>
@@ -5283,7 +5427,7 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B62"/>
       <c r="C62" s="2">
@@ -5295,7 +5439,7 @@
         <v>0.27999999999999992</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F62" s="2">
         <v>0.5</v>
@@ -5322,25 +5466,25 @@
         <v>0</v>
       </c>
       <c r="P62" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q62" s="18" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="R62" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T62" s="1" t="b">
         <f>J62=[1]params_testeithink!J62</f>
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C63" s="2">
         <f t="shared" si="11"/>
@@ -5351,7 +5495,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F63" s="2">
         <v>3</v>
@@ -5379,18 +5523,23 @@
       <c r="P63" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R63"/>
+      <c r="Q63" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R63" t="s">
+        <v>256</v>
+      </c>
       <c r="T63" s="1" t="b">
         <f>J63=[1]params_testeithink!J63</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C64" s="2">
         <f t="shared" si="11"/>
@@ -5401,7 +5550,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F64" s="2">
         <v>3</v>
@@ -5429,18 +5578,23 @@
       <c r="P64" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R64"/>
+      <c r="Q64" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R64" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="T64" s="1" t="b">
         <f>J64=[1]params_testeithink!J64</f>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C65" s="2">
         <f t="shared" si="11"/>
@@ -5451,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F65" s="2">
         <v>3</v>
@@ -5479,18 +5633,23 @@
       <c r="P65" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R65"/>
+      <c r="Q65" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R65" s="17" t="s">
+        <v>256</v>
+      </c>
       <c r="T65" s="1" t="b">
         <f>J65=[1]params_testeithink!J65</f>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C66" s="12">
         <f t="shared" si="11"/>
@@ -5501,7 +5660,7 @@
         <v>0.15</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F66" s="2">
         <v>5</v>
@@ -5529,23 +5688,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P66" s="1" t="s">
-        <v>39</v>
+      <c r="P66" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q66" s="18" t="s">
+        <v>254</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="T66" s="1" t="b">
         <f>J66=[1]params_testeithink!J66</f>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C67" s="12">
         <f t="shared" si="11"/>
@@ -5556,7 +5718,7 @@
         <v>0.15</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F67" s="2">
         <v>5</v>
@@ -5584,21 +5746,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P67" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R67"/>
+      <c r="P67" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q67" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="R67" t="s">
+        <v>229</v>
+      </c>
       <c r="T67" s="1" t="b">
         <f>J67=[1]params_testeithink!J67</f>
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C68" s="12">
         <f t="shared" si="11"/>
@@ -5609,7 +5776,7 @@
         <v>0.15</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F68" s="2">
         <v>5</v>
@@ -5637,21 +5804,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P68" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R68"/>
+      <c r="P68" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q68" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="R68" s="17" t="s">
+        <v>229</v>
+      </c>
       <c r="T68" s="1" t="b">
         <f>J68=[1]params_testeithink!J68</f>
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C69" s="2">
         <f t="shared" si="11"/>
@@ -5698,21 +5870,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P69" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R69"/>
+      <c r="P69" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q69" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="R69" t="s">
+        <v>261</v>
+      </c>
       <c r="T69" s="1" t="b">
         <f>J69=[1]params_testeithink!J69</f>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C70" s="2">
         <f t="shared" si="11"/>
@@ -5759,21 +5936,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="P70" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R70"/>
+      <c r="P70" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q70" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="R70" t="s">
+        <v>229</v>
+      </c>
       <c r="T70" s="1" t="b">
         <f>J70=[1]params_testeithink!J70</f>
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C71" s="2">
         <f t="shared" si="11"/>
@@ -5820,21 +6002,26 @@
         <f t="shared" ref="O71:O78" si="14">D71&gt;C69</f>
         <v>1</v>
       </c>
-      <c r="P71" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R71"/>
+      <c r="P71" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q71" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="R71" s="17" t="s">
+        <v>229</v>
+      </c>
       <c r="T71" s="1" t="b">
         <f>J71=[1]params_testeithink!J71</f>
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C72" s="2">
         <f t="shared" si="11"/>
@@ -5873,21 +6060,26 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="P72" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R72"/>
+      <c r="P72" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q72" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="R72" s="17" t="s">
+        <v>262</v>
+      </c>
       <c r="T72" s="1" t="b">
         <f>J72=[1]params_testeithink!J72</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C73" s="2">
         <f t="shared" si="11"/>
@@ -5926,21 +6118,26 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="P73" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R73"/>
+      <c r="P73" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q73" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="R73" t="s">
+        <v>229</v>
+      </c>
       <c r="T73" s="1" t="b">
         <f>J73=[1]params_testeithink!J73</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C74" s="2">
         <f t="shared" si="11"/>
@@ -5979,10 +6176,15 @@
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="P74" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R74"/>
+      <c r="P74" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q74" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="R74" t="s">
+        <v>229</v>
+      </c>
       <c r="T74" s="1" t="b">
         <f>J74=[1]params_testeithink!J74</f>
         <v>0</v>
@@ -5990,10 +6192,10 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C75" s="7">
         <f t="shared" si="11"/>
@@ -6004,7 +6206,7 @@
         <v>107000</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F75" s="7">
         <v>0.5</v>
@@ -6038,13 +6240,13 @@
         <v>1</v>
       </c>
       <c r="P75" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q75" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R75" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="T75" s="1" t="b">
         <f>J75=[1]params_testeithink!J75</f>
@@ -6053,10 +6255,10 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C76" s="7">
         <f t="shared" si="11"/>
@@ -6067,7 +6269,7 @@
         <v>107000</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F76" s="7">
         <v>0.5</v>
@@ -6101,13 +6303,13 @@
         <v>1</v>
       </c>
       <c r="P76" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q76" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R76" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T76" s="1" t="b">
         <f>J76=[1]params_testeithink!J76</f>
@@ -6116,10 +6318,10 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C77" s="7">
         <f t="shared" si="11"/>
@@ -6130,7 +6332,7 @@
         <v>107000</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F77" s="7">
         <v>0.5</v>
@@ -6164,13 +6366,13 @@
         <v>0</v>
       </c>
       <c r="P77" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q77" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R77" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T77" s="1" t="b">
         <f>J77=[1]params_testeithink!J77</f>
@@ -6179,10 +6381,10 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C78" s="7">
         <f t="shared" si="11"/>
@@ -6193,7 +6395,7 @@
         <v>107000</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F78" s="7">
         <v>0.5</v>
@@ -6227,13 +6429,13 @@
         <v>0</v>
       </c>
       <c r="P78" s="18" t="s">
-        <v>233</v>
+        <v>260</v>
       </c>
       <c r="Q78" s="18" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="R78" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="T78" s="1" t="b">
         <f>J78=[1]params_testeithink!J78</f>
@@ -6242,10 +6444,10 @@
     </row>
     <row r="79" spans="1:20" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C79" s="2">
         <f t="shared" si="11"/>
@@ -6283,20 +6485,23 @@
       <c r="P79" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q79" s="17" t="s">
+        <v>264</v>
+      </c>
       <c r="R79" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="T79" s="1" t="b">
         <f>J79=[1]params_testeithink!J79</f>
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C80" s="2">
         <f t="shared" si="11"/>
@@ -6307,7 +6512,7 @@
         <v>15</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F80" s="2">
         <v>2</v>
@@ -6334,19 +6539,19 @@
       <c r="P80" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="Q80" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="T80" s="1" t="b">
         <f>J80=[1]params_testeithink!J80</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T80" xr:uid="{DA22CF81-2CA1-4C04-ACDB-DC4BF7E98F20}">
-    <filterColumn colId="8">
-      <filters>
-        <filter val="Fixo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:T80" xr:uid="{DA22CF81-2CA1-4C04-ACDB-DC4BF7E98F20}"/>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6371,16 +6576,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6443,25 +6648,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6524,13 +6729,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6569,140 +6774,140 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
         <v>195</v>
-      </c>
-      <c r="B1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D9" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D12" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -6738,7 +6943,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B2">
         <v>250</v>
@@ -6750,7 +6955,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B3">
         <v>10000</v>
@@ -6762,7 +6967,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B4">
         <v>10000</v>
@@ -6774,7 +6979,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B5">
         <v>10000</v>
@@ -6786,7 +6991,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B6">
         <v>10000</v>
@@ -6798,7 +7003,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B7">
         <v>-2</v>

</xml_diff>

<commit_message>
rodando no windows, ok
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -1784,7 +1784,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AMJ80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
@@ -6568,8 +6568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6610,11 +6610,26 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
       <c r="D3">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.9</v>
+      </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
       <c r="D4">
         <v>0.15</v>
       </c>

</xml_diff>

<commit_message>
análise dos resultados com teste t
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_opcao1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,6 +48,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">params!$A$1:$T$80</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">params!$A$1:$T$80</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">params!$A$1:$T$80</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">params!$A$1:$T$80</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="TesteOutroNome" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="TesteOutroNome2" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
@@ -81,6 +82,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1641,33 +1643,33 @@
   </sheetPr>
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="6.3469387755102"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.78061224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.64285714285714"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="43.8724489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -6427,11 +6429,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6512,11 +6513,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -6607,7 +6608,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,11 +6657,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6819,14 +6819,13 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6905,10 +6904,10 @@
         <v>264</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-2</v>
+        <v>-0.5</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -6935,10 +6934,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>